<commit_message>
Player Controller except mixube
</commit_message>
<xml_diff>
--- a/Assets/Resources/CharacterInfo.xlsx
+++ b/Assets/Resources/CharacterInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nhc33\Desktop\Develope\CovergenceProject\YourParfait\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CEAC25-0DD8-4E29-95F8-0E3494554BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C7462B-5853-4B45-AA20-FDF1F401B625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5790" yWindow="3480" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -116,6 +116,150 @@
   </si>
   <si>
     <t>tyneya</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qskill</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wskill</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eskill</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지정한 적에게 나비를 날려 200의 데미지를 입힌다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 마나를 소모하여 가로축으로 강력함 빔을 말사한다. 소모한 마나 만큼 데미지를 입힌다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지정한 대상에게 마석을 던져 200의 피해를 입힌다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5초동안 자신에게 200의 보호막을 부여한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">지정한 방향에 마석을 대량으로 던져서 400의 피해를 입힌다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>와인을 뿌려 200의 피해를 입힌다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>와인을 자신에게 부어 체력을 150 회복한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4초동안 영역을 전개하고 이후 주변의 적에게 100의 피해를 입힌다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신의 공격 데미지를 영구적으로 1% 늘린다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에피타이저의 쿨타임을 초기화 한다. 에피타이저의 재사용 피해를 두배로 늘린다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신의 이동 속도를 5초간 20% 늘린다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QskillName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WskillName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EskillName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간을 달리는 나비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나는 마녀로소이다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리첸시아의 파수꾼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에피타이저</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 디쉬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>디저트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아트르빈식 협상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완벽한 계산</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마석 대폭발</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공간을 가르는 나방</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이름은 아직 없다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홍백의 마녀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다가오지마</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여유로운 한잔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전조강림</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력의 절반을 소모하여 10초동안 평타 데미지를 50% 증가시킨다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신의 이동속도를 영구적으로 2% 증가시킨다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스킬에 따라오는 기본 공격은 100의 추가피해를 입힌다. 더불어 데미지의 50% 만큼 회복한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지정한 방향으로 포크를 날린다. 적중시 표식을 남기며 200의 피해를 입히고, 사거리 내로 재사용시 즉시 적에게 이동한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -123,7 +267,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +277,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -159,8 +312,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -441,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -453,9 +607,13 @@
     <col min="2" max="2" width="16.875" customWidth="1"/>
     <col min="3" max="3" width="27.25" customWidth="1"/>
     <col min="4" max="4" width="19.75" customWidth="1"/>
+    <col min="5" max="5" width="103.5" customWidth="1"/>
+    <col min="6" max="6" width="50.875" customWidth="1"/>
+    <col min="7" max="7" width="80.75" customWidth="1"/>
+    <col min="8" max="10" width="53.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,8 +626,26 @@
       <c r="D1" t="s">
         <v>17</v>
       </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -482,8 +658,26 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -496,8 +690,26 @@
       <c r="D3" t="s">
         <v>19</v>
       </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -510,8 +722,26 @@
       <c r="D4" t="s">
         <v>20</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -524,8 +754,26 @@
       <c r="D5" t="s">
         <v>21</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -537,6 +785,24 @@
       </c>
       <c r="D6" t="s">
         <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>